<commit_message>
Backup projetos da rede neural pra algumas frequências
</commit_message>
<xml_diff>
--- a/Arquivos/Excel/resultados_multicore.xlsx
+++ b/Arquivos/Excel/resultados_multicore.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Desktop\GitDesk\Arquivos\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F80262-8BE5-43BE-A297-8DD53B964350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A0C58B-22AD-4C85-BB01-82DFB355D66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="483" xr2:uid="{7C13D048-D369-4CF7-941B-2AB5863FD600}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="483" activeTab="1" xr2:uid="{7C13D048-D369-4CF7-941B-2AB5863FD600}"/>
   </bookViews>
   <sheets>
     <sheet name="SSF" sheetId="7" r:id="rId1"/>
+    <sheet name="RN" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>clocks</t>
   </si>
@@ -83,12 +84,18 @@
   <si>
     <t>MLT -1 (in)</t>
   </si>
+  <si>
+    <t>Tempo de Atraso [ns]</t>
+  </si>
+  <si>
+    <t>1 pulso</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,6 +219,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5905,8 +5927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7955FCB8-867E-43F2-8076-D8AB814E01C6}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7299,4 +7321,866 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B442ED4B-69CD-429B-93EE-E4EE92BF073B}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>320</v>
+      </c>
+      <c r="C2" s="1">
+        <f>1/B2*1000000</f>
+        <v>3125</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="e">
+        <f>ROUNDUP(E2/D2,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I2">
+        <f>1/J2*1000000</f>
+        <v>320</v>
+      </c>
+      <c r="J2" s="12">
+        <f>ROUNDUP(C2,0)</f>
+        <v>3125</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>400</v>
+      </c>
+      <c r="C3" s="1">
+        <f>1/B3*1000000</f>
+        <v>2500</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15" t="e">
+        <f t="shared" ref="H3:H23" si="0">ROUNDUP(E3/D3,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I23" si="1">1/J3*1000000</f>
+        <v>400</v>
+      </c>
+      <c r="J3" s="12">
+        <f>ROUNDUP(C3,0)</f>
+        <v>2500</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>480</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C23" si="2">1/B4*1000000</f>
+        <v>2083.3333333333335</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>479.84644913627636</v>
+      </c>
+      <c r="J4" s="12">
+        <f>ROUNDUP(C4,0)</f>
+        <v>2084</v>
+      </c>
+      <c r="K4" s="12">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>560</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="2"/>
+        <v>1785.7142857142856</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>559.91041433370663</v>
+      </c>
+      <c r="J5" s="12">
+        <f>ROUNDUP(C5,0)</f>
+        <v>1786</v>
+      </c>
+      <c r="K5" s="12">
+        <v>3</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>640</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="2"/>
+        <v>1562.5</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>639.79526551503511</v>
+      </c>
+      <c r="J6" s="12">
+        <f>ROUNDUP(C6,0)</f>
+        <v>1563</v>
+      </c>
+      <c r="K6" s="12">
+        <v>4</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>720</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="2"/>
+        <v>1388.8888888888889</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>719.94240460763137</v>
+      </c>
+      <c r="J7" s="12">
+        <f>ROUNDUP(C7,0)</f>
+        <v>1389</v>
+      </c>
+      <c r="K7" s="12">
+        <v>5</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>800</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>1250</v>
+      </c>
+      <c r="D8" s="18">
+        <v>25</v>
+      </c>
+      <c r="E8" s="17">
+        <v>925</v>
+      </c>
+      <c r="F8" s="1">
+        <v>926.25</v>
+      </c>
+      <c r="G8" s="14">
+        <v>31.25</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="J8" s="12">
+        <f>ROUNDUP(C8,0)</f>
+        <v>1250</v>
+      </c>
+      <c r="K8" s="12">
+        <v>6</v>
+      </c>
+      <c r="L8" s="7">
+        <v>25980</v>
+      </c>
+      <c r="M8" s="8">
+        <v>222</v>
+      </c>
+      <c r="N8" s="10">
+        <v>38074016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>880</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>1136.3636363636363</v>
+      </c>
+      <c r="D9" s="18">
+        <v>25.013999999999999</v>
+      </c>
+      <c r="E9" s="17">
+        <v>850.476</v>
+      </c>
+      <c r="F9" s="1">
+        <v>851.61300000000006</v>
+      </c>
+      <c r="G9" s="14">
+        <v>30.699000000000002</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>879.50747581354449</v>
+      </c>
+      <c r="J9" s="12">
+        <f>ROUNDUP(C9,0)</f>
+        <v>1137</v>
+      </c>
+      <c r="K9" s="12">
+        <v>7</v>
+      </c>
+      <c r="L9" s="7">
+        <v>21102</v>
+      </c>
+      <c r="M9" s="8">
+        <v>204</v>
+      </c>
+      <c r="N9" s="10">
+        <v>35037580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>960</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>1041.6666666666667</v>
+      </c>
+      <c r="D10" s="18">
+        <v>25.007999999999999</v>
+      </c>
+      <c r="E10" s="17">
+        <v>794.00400000000002</v>
+      </c>
+      <c r="F10" s="1">
+        <v>801.298</v>
+      </c>
+      <c r="G10" s="14">
+        <v>30.218</v>
+      </c>
+      <c r="H10" s="15">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>959.69289827255272</v>
+      </c>
+      <c r="J10" s="12">
+        <f>ROUNDUP(C10,0)</f>
+        <v>1042</v>
+      </c>
+      <c r="K10" s="12">
+        <v>8</v>
+      </c>
+      <c r="L10" s="7">
+        <v>19803</v>
+      </c>
+      <c r="M10" s="8">
+        <v>192</v>
+      </c>
+      <c r="N10" s="10">
+        <v>32980040</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1040</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>961.53846153846155</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1039.5010395010395</v>
+      </c>
+      <c r="J11" s="12">
+        <f>ROUNDUP(C11,0)</f>
+        <v>962</v>
+      </c>
+      <c r="K11" s="12">
+        <v>9</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1120</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>892.85714285714278</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>1119.8208286674133</v>
+      </c>
+      <c r="J12" s="12">
+        <f>ROUNDUP(C12,0)</f>
+        <v>893</v>
+      </c>
+      <c r="K12" s="12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>833.33333333333337</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1199.0407673860911</v>
+      </c>
+      <c r="J13" s="12">
+        <f>ROUNDUP(C13,0)</f>
+        <v>834</v>
+      </c>
+      <c r="K13" s="12">
+        <v>11</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1280</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>781.25</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>1278.7723785166243</v>
+      </c>
+      <c r="J14" s="12">
+        <f>ROUNDUP(C14,0)</f>
+        <v>782</v>
+      </c>
+      <c r="K14" s="12">
+        <v>12</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1360</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>735.29411764705878</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>1358.695652173913</v>
+      </c>
+      <c r="J15" s="12">
+        <f>ROUNDUP(C15,0)</f>
+        <v>736</v>
+      </c>
+      <c r="K15" s="12">
+        <v>13</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1440</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>694.44444444444446</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>1438.8489208633093</v>
+      </c>
+      <c r="J16" s="12">
+        <f>ROUNDUP(C16,0)</f>
+        <v>695</v>
+      </c>
+      <c r="K16" s="12">
+        <v>14</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1520</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>657.8947368421052</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>1519.7568389057751</v>
+      </c>
+      <c r="J17" s="12">
+        <f>ROUNDUP(C17,0)</f>
+        <v>658</v>
+      </c>
+      <c r="K17" s="12">
+        <v>15</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>625</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+      <c r="J18" s="12">
+        <f>ROUNDUP(C18,0)</f>
+        <v>625</v>
+      </c>
+      <c r="K18" s="12">
+        <v>16</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1680</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>595.2380952380953</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>1677.8523489932886</v>
+      </c>
+      <c r="J19" s="12">
+        <f>ROUNDUP(C19,0)</f>
+        <v>596</v>
+      </c>
+      <c r="K19" s="12">
+        <v>17</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1760</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>568.18181818181813</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>1757.4692442882249</v>
+      </c>
+      <c r="J20" s="12">
+        <f>ROUNDUP(C20,0)</f>
+        <v>569</v>
+      </c>
+      <c r="K20" s="12">
+        <v>18</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1840</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>543.47826086956525</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>1838.2352941176471</v>
+      </c>
+      <c r="J21" s="12">
+        <f>ROUNDUP(C21,0)</f>
+        <v>544</v>
+      </c>
+      <c r="K21" s="12">
+        <v>19</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1920</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="2"/>
+        <v>520.83333333333337</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>1919.3857965451054</v>
+      </c>
+      <c r="J22" s="12">
+        <f>ROUNDUP(C22,0)</f>
+        <v>521</v>
+      </c>
+      <c r="K22" s="12">
+        <v>20</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="J23" s="12">
+        <f>ROUNDUP(C23,0)</f>
+        <v>500</v>
+      </c>
+      <c r="K23" s="12">
+        <v>21</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>